<commit_message>
trail-ran with Feb, Mar and Apr - small debugging - also save RData from 05_track-metrics - finalised gitignore (data folder)
</commit_message>
<xml_diff>
--- a/outputs/status_rel-202303.xlsx
+++ b/outputs/status_rel-202303.xlsx
@@ -388,19 +388,19 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0.00411522633744856</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0.2071330589849108</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.2208504801097394</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.2043895747599451</v>
+        <v>0.72</v>
       </c>
       <c r="E2">
-        <v>0.186556927297668</v>
+        <v>13.32</v>
       </c>
     </row>
   </sheetData>
@@ -410,7 +410,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,30 +419,35 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>STATE.NAME</t>
+          <t>STATE.CODE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>CONCERN.1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>CONCERN.2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>CONCERN.3</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>CONCERN.4</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>CONCERN.5</t>
         </is>
@@ -451,77 +456,94 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>IN-BR</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Bihar</t>
         </is>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
       <c r="C2">
-        <v>0.02631578947368421</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.07894736842105263</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.1578947368421053</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.7631578947368421</v>
+        <v>3.23</v>
+      </c>
+      <c r="G2">
+        <v>54.84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>0</v>
+          <t>IN-DD</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Daman and Diu</t>
+        </is>
       </c>
       <c r="C3">
-        <v>0.08333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.08333333333333333</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.5416666666666666</v>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>0</v>
+          <t>IN-JH</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Jharkhand</t>
+        </is>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>47.37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Puducherry</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>0</v>
+          <t>IN-MN</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Manipur</t>
+        </is>
       </c>
       <c r="C5">
         <v>0</v>
@@ -530,625 +552,444 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>30.77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mizoram</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>0</v>
+          <t>IN-UP</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
       </c>
       <c r="C6">
-        <v>0.1818181818181818</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0.1818181818181818</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.1818181818181818</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.4545454545454545</v>
+        <v>1.49</v>
+      </c>
+      <c r="G6">
+        <v>29.85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>0</v>
+          <t>IN-MZ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mizoram</t>
+        </is>
       </c>
       <c r="C7">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.1866666666666667</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.28</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.4533333333333333</v>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>27.27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>IN-AR</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Arunachal Pradesh</t>
         </is>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
       <c r="C8">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.4</v>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Nagaland</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>0</v>
+          <t>IN-OR</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
       </c>
       <c r="C9">
-        <v>0.09090909090909091</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.4545454545454545</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.09090909090909091</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.3636363636363636</v>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>18.52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Manipur</t>
-        </is>
-      </c>
-      <c r="B10">
-        <v>0</v>
+          <t>IN-ML</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Meghalaya</t>
+        </is>
       </c>
       <c r="C10">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0.3125</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0.3125</v>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>18.18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>IN-PB</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>Punjab</t>
         </is>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
       <c r="C11">
-        <v>0.09090909090909091</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.2272727272727273</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.4090909090909091</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0.2727272727272727</v>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>14.29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Odisha</t>
-        </is>
-      </c>
-      <c r="B12">
-        <v>0</v>
+          <t>IN-HR</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
       </c>
       <c r="C12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>0.2666666666666667</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.3666666666666666</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.1666666666666667</v>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>13.64</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>IN-TS</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>Telangana</t>
         </is>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
       <c r="C13">
-        <v>0.2424242424242424</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0.2121212121212121</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0.1515151515151515</v>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>12.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Tripura</t>
-        </is>
-      </c>
-      <c r="B14">
-        <v>0</v>
+          <t>IN-AS</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Assam</t>
+        </is>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0.125</v>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>12.12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
-        </is>
-      </c>
-      <c r="B15">
-        <v>0.09090909090909091</v>
+          <t>IN-MP</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Madhya Pradesh</t>
+        </is>
       </c>
       <c r="C15">
-        <v>0.3636363636363636</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0.5454545454545454</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0.09090909090909091</v>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>11.54</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-      <c r="B16">
-        <v>0</v>
+          <t>IN-NL</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Nagaland</t>
+        </is>
       </c>
       <c r="C16">
-        <v>0.1818181818181818</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0.2727272727272727</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0.4545454545454545</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0.09090909090909091</v>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
-        </is>
-      </c>
-      <c r="B17">
-        <v>0</v>
+          <t>IN-RJ</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
       </c>
       <c r="C17">
-        <v>0.09090909090909091</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0.4090909090909091</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0.4090909090909091</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0.09090909090909091</v>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>6.06</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Haryana</t>
-        </is>
-      </c>
-      <c r="B18">
-        <v>0</v>
+          <t>IN-MH</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Maharashtra</t>
+        </is>
       </c>
       <c r="C18">
-        <v>0.1363636363636364</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0.4090909090909091</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0.3636363636363636</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0.09090909090909091</v>
+        <v>2.78</v>
+      </c>
+      <c r="G18">
+        <v>5.56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="B19">
-        <v>0.0303030303030303</v>
+          <t>IN-JK</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Jammu and Kashmir</t>
+        </is>
       </c>
       <c r="C19">
-        <v>0.2121212121212121</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0.303030303030303</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0.1818181818181818</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.09090909090909091</v>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>4.76</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
-        </is>
-      </c>
-      <c r="B20">
-        <v>0</v>
+          <t>IN-WB</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>West Bengal</t>
+        </is>
       </c>
       <c r="C20">
-        <v>0.1153846153846154</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0.4038461538461539</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0.3461538461538461</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0.07692307692307693</v>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>4.35</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>West Bengal</t>
-        </is>
-      </c>
-      <c r="B21">
-        <v>0</v>
+          <t>IN-CT</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Chhattisgarh</t>
+        </is>
       </c>
       <c r="C21">
-        <v>0.3478260869565217</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0.2608695652173913</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0.08695652173913043</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0.04347826086956522</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Chhattisgarh</t>
-        </is>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0.2592592592592592</v>
-      </c>
-      <c r="D22">
-        <v>0.4074074074074074</v>
-      </c>
-      <c r="E22">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="F22">
-        <v>0.03703703703703703</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Rajasthan</t>
-        </is>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0.303030303030303</v>
-      </c>
-      <c r="D23">
-        <v>0.303030303030303</v>
-      </c>
-      <c r="E23">
-        <v>0.1818181818181818</v>
-      </c>
-      <c r="F23">
-        <v>0.0303030303030303</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Himachal Pradesh</t>
-        </is>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0.4166666666666667</v>
-      </c>
-      <c r="D24">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="E24">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Gujarat</t>
-        </is>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0.5454545454545454</v>
-      </c>
-      <c r="D25">
-        <v>0.09090909090909091</v>
-      </c>
-      <c r="E25">
-        <v>0.06060606060606061</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Maharashtra</t>
-        </is>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0.3055555555555556</v>
-      </c>
-      <c r="D26">
-        <v>0.1944444444444444</v>
-      </c>
-      <c r="E26">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0.3</v>
-      </c>
-      <c r="D27">
-        <v>0.06666666666666667</v>
-      </c>
-      <c r="E27">
-        <v>0.03333333333333333</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Tamil Nadu</t>
-        </is>
-      </c>
-      <c r="B28">
-        <v>0.02702702702702703</v>
-      </c>
-      <c r="C28">
-        <v>0.4324324324324325</v>
-      </c>
-      <c r="D28">
-        <v>0.05405405405405406</v>
-      </c>
-      <c r="E28">
-        <v>0.02702702702702703</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Chandigarh</t>
-        </is>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Dadra and Nagar Haveli</t>
-        </is>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Andhra Pradesh</t>
-        </is>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>0.5384615384615384</v>
-      </c>
-      <c r="D31">
-        <v>0.1538461538461539</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Uttarakhand</t>
-        </is>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0.2307692307692308</v>
-      </c>
-      <c r="D32">
-        <v>0.07692307692307693</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Ladakh</t>
-        </is>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0.5</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
+        <v>7.41</v>
+      </c>
+      <c r="G21">
         <v>0</v>
       </c>
     </row>
@@ -1207,16 +1048,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.02222222222222222</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.06666666666666667</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.1777777777777778</v>
+        <v>2.7</v>
       </c>
       <c r="F2">
-        <v>0.7555555555555555</v>
+        <v>45.95</v>
       </c>
     </row>
     <row r="3">
@@ -1226,19 +1067,19 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.01739130434782609</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.1652173913043478</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.2521739130434782</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.2347826086956522</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.2521739130434782</v>
+        <v>18.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>